<commit_message>
Robinson common neutral vs common DS
</commit_message>
<xml_diff>
--- a/result_datasets/Robinson_Permutation_importance_signs.xlsx
+++ b/result_datasets/Robinson_Permutation_importance_signs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="80">
   <si>
     <t>mean</t>
   </si>
@@ -40,79 +40,214 @@
     <t>sign coef</t>
   </si>
   <si>
+    <t>geneLen</t>
+  </si>
+  <si>
     <t>median_IUPRED</t>
   </si>
   <si>
+    <t>IDR ratio</t>
+  </si>
+  <si>
+    <t>cai</t>
+  </si>
+  <si>
     <t>A3D mean score</t>
   </si>
   <si>
-    <t>cai</t>
+    <t>A3D ratio</t>
+  </si>
+  <si>
+    <t>Imputed log2(MS)</t>
+  </si>
+  <si>
+    <t>Intron</t>
+  </si>
+  <si>
+    <t>Hydrophobic AA%</t>
+  </si>
+  <si>
+    <t>codonBias</t>
+  </si>
+  <si>
+    <t>Cytoplasmic Ribosomal Proteins_WP210</t>
+  </si>
+  <si>
+    <t>RNA binding (GO:0003723)</t>
+  </si>
+  <si>
+    <t>translation (GO:0006412)</t>
+  </si>
+  <si>
+    <t>ncRNA processing (GO:0034470)</t>
   </si>
   <si>
     <t>%Helical</t>
   </si>
   <si>
-    <t>geneLen</t>
-  </si>
-  <si>
-    <t>aliphaticIndex</t>
+    <t>small-subunit processome (GO:0032040)</t>
+  </si>
+  <si>
+    <t>ribosomal large subunit binding (GO:0043023)</t>
+  </si>
+  <si>
+    <t>mitotic spindle checkpoint (GO:0071174)</t>
+  </si>
+  <si>
+    <t>P-body (GO:0000932)</t>
+  </si>
+  <si>
+    <t>negative regulation of chromatin organization (GO:1905268)</t>
+  </si>
+  <si>
+    <t>Serine/threonine-specific protein phosphatase/bis(5-nucleosyl)-tetraphosphatase</t>
+  </si>
+  <si>
+    <t>mitotic spindle elongation (GO:0000022)</t>
   </si>
   <si>
     <t>gravyScore</t>
   </si>
   <si>
-    <t>A3D ratio</t>
-  </si>
-  <si>
-    <t>Charged AA%</t>
+    <t>GDP-dissociation inhibitor activity (GO:0005092)</t>
+  </si>
+  <si>
+    <t>Nutrient control of ribosomal gene expression_WP2869</t>
+  </si>
+  <si>
+    <t>Glucose Repression_WP2836</t>
+  </si>
+  <si>
+    <t>GTP binding (GO:0005525)</t>
+  </si>
+  <si>
+    <t>purine ribonucleoside binding (GO:0032550)</t>
+  </si>
+  <si>
+    <t>guanyl ribonucleotide binding (GO:0032561)</t>
+  </si>
+  <si>
+    <t>PSIPRED_coil</t>
+  </si>
+  <si>
+    <t>cytoplasmic ribonucleoprotein granule (GO:0036464)</t>
+  </si>
+  <si>
+    <t>cytosolic small ribosomal subunit (GO:0022627)</t>
+  </si>
+  <si>
+    <t>preribosome, large subunit precursor (GO:0030687)</t>
+  </si>
+  <si>
+    <t>regulation of intracellular transport (GO:0032386)</t>
+  </si>
+  <si>
+    <t>purine ribonucleoside triphosphate binding (GO:0035639)</t>
+  </si>
+  <si>
+    <t>cytoplasmic translational initiation (GO:0002183)</t>
+  </si>
+  <si>
+    <t>cytosolic part (GO:0044445)</t>
+  </si>
+  <si>
+    <t>ribosome assembly (GO:0042255)</t>
+  </si>
+  <si>
+    <t>regulation of DNA-templated transcription in response to stress (GO:0043620)</t>
+  </si>
+  <si>
+    <t>rRNA-containing ribonucleoprotein complex export from nucleus (GO:0071428)</t>
+  </si>
+  <si>
+    <t>microtubule cytoskeleton (GO:0015630)</t>
+  </si>
+  <si>
+    <t>hydrogen-exporting ATPase activity (GO:0036442)</t>
+  </si>
+  <si>
+    <t>maturation of SSU-rRNA from tricistronic rRNA transcript (SSU-rRNA, 5.8S rRNA, LSU-rRNA) (GO:0000462)</t>
+  </si>
+  <si>
+    <t>Pleckstrin homology domain</t>
+  </si>
+  <si>
+    <t>cellular protein complex disassembly (GO:0043624)</t>
+  </si>
+  <si>
+    <t>positive regulation of cytokinesis, actomyosin contractile ring assembly (GO:2000433)</t>
+  </si>
+  <si>
+    <t>regulation of mitotic actomyosin contractile ring assembly (GO:1903499)</t>
+  </si>
+  <si>
+    <t>positive regulation of mitotic actomyosin contractile ring assembly (GO:1903501)</t>
+  </si>
+  <si>
+    <t>adenyl ribonucleotide binding (GO:0032559)</t>
+  </si>
+  <si>
+    <t>RNA export from nucleus (GO:0006405)</t>
+  </si>
+  <si>
+    <t>tRNA transport (GO:0051031)</t>
+  </si>
+  <si>
+    <t>90S preribosome (GO:0030686)</t>
+  </si>
+  <si>
+    <t>RNA transport (GO:0050658)</t>
+  </si>
+  <si>
+    <t>Myb domain</t>
+  </si>
+  <si>
+    <t>establishment of protein localization to organelle (GO:0072594)</t>
+  </si>
+  <si>
+    <t>protein import (GO:0017038)</t>
+  </si>
+  <si>
+    <t>multi-eIF complex (GO:0043614)</t>
+  </si>
+  <si>
+    <t>oxysterol binding (GO:0008142)</t>
+  </si>
+  <si>
+    <t>sterol transporter activity (GO:0015248)</t>
+  </si>
+  <si>
+    <t>sterol binding (GO:0032934)</t>
+  </si>
+  <si>
+    <t>prions</t>
+  </si>
+  <si>
+    <t>Glycolysis and Gluconeogenesis_WP515</t>
   </si>
   <si>
     <t>aromaticityScore</t>
   </si>
   <si>
-    <t>IDR ratio</t>
-  </si>
-  <si>
-    <t>Intron</t>
-  </si>
-  <si>
-    <t>Hydrophobic AA%</t>
-  </si>
-  <si>
-    <t>Cytoplasmic Ribosomal Proteins_WP210</t>
+    <t>cellular macromolecule biosynthetic process (GO:0034645)</t>
   </si>
   <si>
     <t>ribosome biogenesis (GO:0042254)</t>
   </si>
   <si>
-    <t>translation (GO:0006412)</t>
-  </si>
-  <si>
-    <t>ncRNA processing (GO:0034470)</t>
-  </si>
-  <si>
-    <t>maturation of SSU-rRNA from tricistronic rRNA transcript (SSU-rRNA, 5.8S rRNA, LSU-rRNA) (GO:0000462)</t>
-  </si>
-  <si>
-    <t>ribosomal large subunit binding (GO:0043023)</t>
-  </si>
-  <si>
-    <t>purine ribonucleoside triphosphate binding (GO:0035639)</t>
-  </si>
-  <si>
-    <t>cytosolic large ribosomal subunit (GO:0022625)</t>
+    <t>ribosome (GO:0005840)</t>
+  </si>
+  <si>
+    <t>positive regulation of transcription, DNA-templated (GO:0045893)</t>
   </si>
   <si>
     <t>cytoplasmic stress granule (GO:0010494)</t>
   </si>
   <si>
-    <t>rRNA processing (GO:0006364)</t>
-  </si>
-  <si>
-    <t>GDP-dissociation inhibitor activity (GO:0005092)</t>
-  </si>
-  <si>
-    <t>RNA helicase activity (GO:0003724)</t>
+    <t>RNAseq Eupl</t>
+  </si>
+  <si>
+    <t>regulation of transcription from RNA polymerase II promoter (GO:0006357)</t>
   </si>
   <si>
     <t>T</t>
@@ -476,7 +611,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -528,43 +663,43 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>0.06531713900134957</v>
+        <v>0.09623100303951362</v>
       </c>
       <c r="C2">
-        <v>0.05927800269905532</v>
+        <v>0.0998784194528875</v>
       </c>
       <c r="D2">
-        <v>0.04095816464237523</v>
+        <v>0.117861482381531</v>
       </c>
       <c r="E2">
-        <v>0.05695006747638326</v>
+        <v>0.1037059538274605</v>
       </c>
       <c r="F2">
-        <v>0.05516194331983811</v>
+        <v>0.09416767922235725</v>
       </c>
       <c r="G2">
-        <v>0.0555330634278003</v>
+        <v>0.10236890758475</v>
       </c>
       <c r="H2">
-        <v>0.008053893594876098</v>
+        <v>0.00840171549723623</v>
       </c>
       <c r="I2">
-        <v>2.507189014244825E-09</v>
+        <v>7.711567381474502E-40</v>
       </c>
       <c r="J2">
-        <v>5.96098700902366</v>
+        <v>13.2097151713069</v>
       </c>
       <c r="K2">
-        <v>1.00287560569793E-08</v>
+        <v>1.172158241984124E-38</v>
       </c>
       <c r="L2">
-        <v>-0.8386285239842968</v>
+        <v>1.564143481673576</v>
       </c>
       <c r="M2" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="N2" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -572,43 +707,43 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>0.05192307692307697</v>
+        <v>0.0483282674772036</v>
       </c>
       <c r="C3">
-        <v>0.02473009446693657</v>
+        <v>0.03920972644376898</v>
       </c>
       <c r="D3">
-        <v>0.04858299595141705</v>
+        <v>0.04368165249088701</v>
       </c>
       <c r="E3">
-        <v>0.02611336032388665</v>
+        <v>0.03997569866342648</v>
       </c>
       <c r="F3">
-        <v>0.04008097165991907</v>
+        <v>0.04210206561360878</v>
       </c>
       <c r="G3">
-        <v>0.03828609986504726</v>
+        <v>0.04265948213777897</v>
       </c>
       <c r="H3">
-        <v>0.01119960398715324</v>
+        <v>0.003243275527062988</v>
       </c>
       <c r="I3">
-        <v>4.305252420190502E-10</v>
+        <v>3.124231371028439E-11</v>
       </c>
       <c r="J3">
-        <v>-6.242538688138421</v>
+        <v>6.640593233815991</v>
       </c>
       <c r="K3">
-        <v>2.044994899590488E-09</v>
+        <v>1.582943894654409E-10</v>
       </c>
       <c r="L3">
-        <v>-0.6255611877700662</v>
+        <v>-0.8613362791840599</v>
       </c>
       <c r="M3" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="N3" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -616,43 +751,43 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>0.02850877192982459</v>
+        <v>0.03854103343465039</v>
       </c>
       <c r="C4">
-        <v>0.02871120107962214</v>
+        <v>0.0249848024316109</v>
       </c>
       <c r="D4">
-        <v>0.02462887989203784</v>
+        <v>0.02430133657351156</v>
       </c>
       <c r="E4">
-        <v>0.0157557354925776</v>
+        <v>0.044228432563791</v>
       </c>
       <c r="F4">
-        <v>0.02540485829959519</v>
+        <v>0.028857837181045</v>
       </c>
       <c r="G4">
-        <v>0.02460188933873147</v>
+        <v>0.03218268843692177</v>
       </c>
       <c r="H4">
-        <v>0.004712750790701958</v>
+        <v>0.007880462025721338</v>
       </c>
       <c r="I4">
-        <v>6.537959673269912E-39</v>
+        <v>7.431592592171749E-20</v>
       </c>
       <c r="J4">
-        <v>13.04783430072999</v>
+        <v>9.12117246466835</v>
       </c>
       <c r="K4">
-        <v>1.656283117228378E-37</v>
+        <v>6.275567077833922E-19</v>
       </c>
       <c r="L4">
-        <v>0.6889056230337169</v>
+        <v>0.8026948316772223</v>
       </c>
       <c r="M4" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="N4" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -660,43 +795,43 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>0.0432186234817814</v>
+        <v>0.01434650455927048</v>
       </c>
       <c r="C5">
-        <v>-6.747638326584093E-05</v>
+        <v>0.007355623100303898</v>
       </c>
       <c r="D5">
-        <v>0.01251686909581653</v>
+        <v>0.01530984204131232</v>
       </c>
       <c r="E5">
-        <v>0.02091767881241565</v>
+        <v>0.01366950182260024</v>
       </c>
       <c r="F5">
-        <v>0.004959514170040535</v>
+        <v>0.0388821385176185</v>
       </c>
       <c r="G5">
-        <v>0.01630904183535766</v>
+        <v>0.01791272200822109</v>
       </c>
       <c r="H5">
-        <v>0.01521017962056383</v>
+        <v>0.01085049837247239</v>
       </c>
       <c r="I5">
-        <v>1.296363032978225E-11</v>
+        <v>3.83258718300085E-45</v>
       </c>
       <c r="J5">
-        <v>-6.769043792420788</v>
+        <v>14.09935460128514</v>
       </c>
       <c r="K5">
-        <v>7.578737731257314E-11</v>
+        <v>9.709220863602154E-44</v>
       </c>
       <c r="L5">
-        <v>0.2141559951112787</v>
+        <v>0.5844285182670883</v>
       </c>
       <c r="M5" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="N5" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -704,43 +839,43 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>0.02000674763832661</v>
+        <v>0.008632218844984763</v>
       </c>
       <c r="C6">
-        <v>0.01555330634278003</v>
+        <v>0.01896656534954403</v>
       </c>
       <c r="D6">
-        <v>0.01315789473684217</v>
+        <v>0.02727825030376674</v>
       </c>
       <c r="E6">
-        <v>0.006848852901484482</v>
+        <v>0.007290400972053424</v>
       </c>
       <c r="F6">
-        <v>0.02112010796221326</v>
+        <v>0.01154313487241801</v>
       </c>
       <c r="G6">
-        <v>0.01533738191632931</v>
+        <v>0.01474211406855339</v>
       </c>
       <c r="H6">
-        <v>0.005139937924272187</v>
+        <v>0.007457788089589773</v>
       </c>
       <c r="I6">
-        <v>3.659792641659752E-21</v>
+        <v>4.462014286030985E-09</v>
       </c>
       <c r="J6">
-        <v>9.44192884878043</v>
+        <v>-5.866086371080583</v>
       </c>
       <c r="K6">
-        <v>3.476803009576765E-20</v>
+        <v>1.474404720601543E-08</v>
       </c>
       <c r="L6">
-        <v>0.8033839964495286</v>
+        <v>-0.3980682033000373</v>
       </c>
       <c r="M6" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
       <c r="N6" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -748,43 +883,43 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>0.04406207827260463</v>
+        <v>0.00765957446808504</v>
       </c>
       <c r="C7">
-        <v>-0.0005398110661268496</v>
+        <v>0.01373860182370817</v>
       </c>
       <c r="D7">
-        <v>0.01757759784075578</v>
+        <v>0.02071688942891863</v>
       </c>
       <c r="E7">
-        <v>0.008468286099865052</v>
+        <v>0.006439854191980532</v>
       </c>
       <c r="F7">
-        <v>0.0007422402159244723</v>
+        <v>0.01312272174969625</v>
       </c>
       <c r="G7">
-        <v>0.01406207827260462</v>
+        <v>0.01233552833247773</v>
       </c>
       <c r="H7">
-        <v>0.01633574391830749</v>
+        <v>0.005088398974917258</v>
       </c>
       <c r="I7">
-        <v>6.46266958732979E-05</v>
+        <v>7.874183300704399E-07</v>
       </c>
       <c r="J7">
-        <v>-3.995247526056751</v>
+        <v>-4.938460228488614</v>
       </c>
       <c r="K7">
-        <v>0.0001637209628790213</v>
+        <v>2.216436780939016E-06</v>
       </c>
       <c r="L7">
-        <v>-0.2566848114416372</v>
+        <v>0.4575198513512831</v>
       </c>
       <c r="M7" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="N7" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -792,43 +927,43 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <v>0.006646423751686947</v>
+        <v>0.003829787234042503</v>
       </c>
       <c r="C8">
-        <v>0.04665991902834008</v>
+        <v>0.003343465045592664</v>
       </c>
       <c r="D8">
-        <v>0.003070175438596534</v>
+        <v>0.009538274605103304</v>
       </c>
       <c r="E8">
-        <v>-0.001585695006747634</v>
+        <v>0.004799513973268499</v>
       </c>
       <c r="F8">
-        <v>0.005769230769230837</v>
+        <v>0.00267314702308632</v>
       </c>
       <c r="G8">
-        <v>0.01211201079622135</v>
+        <v>0.004836837576218658</v>
       </c>
       <c r="H8">
-        <v>0.01751024496873847</v>
+        <v>0.002450745678544568</v>
       </c>
       <c r="I8">
-        <v>1.509453565603148E-05</v>
+        <v>7.256228956554362E-43</v>
       </c>
       <c r="J8">
-        <v>-4.327304300713191</v>
+        <v>13.72436478145878</v>
       </c>
       <c r="K8">
-        <v>3.955809344339285E-05</v>
+        <v>1.378683501745329E-41</v>
       </c>
       <c r="L8">
-        <v>-0.2573003136172812</v>
+        <v>0.4154943430126173</v>
       </c>
       <c r="M8" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="N8" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -836,43 +971,37 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <v>0.01352901484480437</v>
+        <v>0.002796352583586592</v>
       </c>
       <c r="C9">
-        <v>0.01244939271255062</v>
+        <v>0.004924012158054669</v>
       </c>
       <c r="D9">
-        <v>0.01217948717948721</v>
+        <v>0.005650060753341468</v>
       </c>
       <c r="E9">
-        <v>0.003103913630229427</v>
+        <v>0.006014580801944091</v>
       </c>
       <c r="F9">
-        <v>0.01467611336032393</v>
+        <v>0.002976913730255215</v>
       </c>
       <c r="G9">
-        <v>0.01118758434547911</v>
+        <v>0.004472384005436407</v>
       </c>
       <c r="H9">
-        <v>0.004137001215626966</v>
-      </c>
-      <c r="I9">
-        <v>1.033337604775325E-05</v>
+        <v>0.001342741534393765</v>
       </c>
       <c r="J9">
-        <v>-4.410077227997325</v>
-      </c>
-      <c r="K9">
-        <v>2.804773498675882E-05</v>
+        <v>1</v>
       </c>
       <c r="L9">
-        <v>0.297780993898809</v>
+        <v>1.3611687525632</v>
       </c>
       <c r="M9" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="N9" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -880,43 +1009,43 @@
         <v>16</v>
       </c>
       <c r="B10">
-        <v>0.02179487179487184</v>
+        <v>0.0003039513677811079</v>
       </c>
       <c r="C10">
-        <v>0.01477732793522267</v>
+        <v>0.002127659574468044</v>
       </c>
       <c r="D10">
-        <v>0.006680161943319896</v>
+        <v>0.02017010935601461</v>
       </c>
       <c r="E10">
-        <v>0.006207827260458843</v>
+        <v>0.0004860267314701683</v>
       </c>
       <c r="F10">
-        <v>0.006376518218623517</v>
+        <v>-0.001579586877278227</v>
       </c>
       <c r="G10">
-        <v>0.01116734143049935</v>
+        <v>0.004301632030491141</v>
       </c>
       <c r="H10">
-        <v>0.006223503061948129</v>
+        <v>0.008020770027749532</v>
       </c>
       <c r="I10">
-        <v>0.02698859537395604</v>
+        <v>4.027529989344609E-05</v>
       </c>
       <c r="J10">
-        <v>2.21168271892416</v>
+        <v>-4.105894661783091</v>
       </c>
       <c r="K10">
-        <v>0.04883650591477759</v>
+        <v>9.275523611823948E-05</v>
       </c>
       <c r="L10">
-        <v>-0.3901972782191109</v>
+        <v>0.07307631737030169</v>
       </c>
       <c r="M10" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
       <c r="N10" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -924,43 +1053,43 @@
         <v>17</v>
       </c>
       <c r="B11">
-        <v>0.02921727395411611</v>
+        <v>0.007598784194528818</v>
       </c>
       <c r="C11">
-        <v>-0.0004723346828609754</v>
+        <v>0.004802431610942204</v>
       </c>
       <c r="D11">
-        <v>0.002192982456140402</v>
+        <v>0.005832320777642774</v>
       </c>
       <c r="E11">
-        <v>-0.002699055330634281</v>
+        <v>0.0001822600243012951</v>
       </c>
       <c r="F11">
-        <v>0.002631578947368463</v>
+        <v>-0.002308626974483563</v>
       </c>
       <c r="G11">
-        <v>0.006174089068825944</v>
+        <v>0.003221433926586306</v>
       </c>
       <c r="H11">
-        <v>0.01168156323186689</v>
+        <v>0.003695825503810661</v>
       </c>
       <c r="I11">
-        <v>2.826601689129093E-09</v>
+        <v>7.559954059576977E-35</v>
       </c>
       <c r="J11">
-        <v>-5.941364010118932</v>
+        <v>12.31458877172889</v>
       </c>
       <c r="K11">
-        <v>1.074108641869055E-08</v>
+        <v>9.575941808797504E-34</v>
       </c>
       <c r="L11">
-        <v>-0.1244333371622994</v>
+        <v>0.2788785367413229</v>
       </c>
       <c r="M11" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="N11" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -968,43 +1097,37 @@
         <v>18</v>
       </c>
       <c r="B12">
-        <v>0.003778677462888014</v>
+        <v>0.001884498480243113</v>
       </c>
       <c r="C12">
-        <v>0.00253036437246964</v>
+        <v>0.004255319148936132</v>
       </c>
       <c r="D12">
-        <v>-0.001248313090418318</v>
+        <v>0.00255164034021873</v>
       </c>
       <c r="E12">
-        <v>0.0135290148448043</v>
+        <v>0.004313487241798275</v>
       </c>
       <c r="F12">
-        <v>0.01140350877192986</v>
+        <v>0.001701093560145839</v>
       </c>
       <c r="G12">
-        <v>0.005998650472334699</v>
+        <v>0.002941207754268418</v>
       </c>
       <c r="H12">
-        <v>0.005574847985979905</v>
-      </c>
-      <c r="I12">
-        <v>4.741543535265521E-14</v>
+        <v>0.001132812449071379</v>
       </c>
       <c r="J12">
-        <v>7.538844388798103</v>
-      </c>
-      <c r="K12">
-        <v>3.603573086801796E-13</v>
+        <v>1</v>
       </c>
       <c r="L12">
-        <v>0.4194551733071387</v>
+        <v>1.021985394430562</v>
       </c>
       <c r="M12" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="N12" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -1012,37 +1135,37 @@
         <v>19</v>
       </c>
       <c r="B13">
-        <v>0.004925775978407598</v>
+        <v>0.003161094224923977</v>
       </c>
       <c r="C13">
-        <v>0.003711201079622128</v>
+        <v>0.0007294832826747477</v>
       </c>
       <c r="D13">
-        <v>0.004790823211875894</v>
+        <v>0.005103280680437449</v>
       </c>
       <c r="E13">
-        <v>0.004588394062078283</v>
+        <v>0.002369380315917358</v>
       </c>
       <c r="F13">
-        <v>0.003373819163292891</v>
+        <v>-0.0001215066828675337</v>
       </c>
       <c r="G13">
-        <v>0.004278002699055359</v>
+        <v>0.002248346364217199</v>
       </c>
       <c r="H13">
-        <v>0.0006193141109626924</v>
+        <v>0.001839649768291257</v>
       </c>
       <c r="J13">
         <v>1</v>
       </c>
       <c r="L13">
-        <v>0.9396987201740273</v>
+        <v>0.5786934619121378</v>
       </c>
       <c r="M13" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="N13" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -1050,43 +1173,37 @@
         <v>20</v>
       </c>
       <c r="B14">
-        <v>0.0003036437246964008</v>
+        <v>0.003768996960486282</v>
       </c>
       <c r="C14">
-        <v>0.01804993252361673</v>
+        <v>0.002492401215805429</v>
       </c>
       <c r="D14">
-        <v>0.001248313090418418</v>
+        <v>-0.0001215066828675337</v>
       </c>
       <c r="E14">
-        <v>-0.001585695006747645</v>
+        <v>0.002247873633049779</v>
       </c>
       <c r="F14">
-        <v>0.001147098515519618</v>
+        <v>-0.0003037667071688621</v>
       </c>
       <c r="G14">
-        <v>0.003832658569500704</v>
+        <v>0.001616799683861019</v>
       </c>
       <c r="H14">
-        <v>0.007181009041872463</v>
-      </c>
-      <c r="I14">
-        <v>0.0003064736900437317</v>
+        <v>0.001581592221564323</v>
       </c>
       <c r="J14">
-        <v>-3.609765714029177</v>
-      </c>
-      <c r="K14">
-        <v>0.0007058181952522305</v>
+        <v>1</v>
       </c>
       <c r="L14">
-        <v>0.07781686941255765</v>
+        <v>0.3943565362416183</v>
       </c>
       <c r="M14" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="N14" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -1094,37 +1211,37 @@
         <v>21</v>
       </c>
       <c r="B15">
-        <v>0.0005060728744939791</v>
+        <v>0.0004255319148935621</v>
       </c>
       <c r="C15">
-        <v>0.00377867746288797</v>
+        <v>0.001580547112461961</v>
       </c>
       <c r="D15">
-        <v>0.002091767881241624</v>
+        <v>0.0008505467800729138</v>
       </c>
       <c r="E15">
-        <v>0.00668016194331984</v>
+        <v>0.002247873633049791</v>
       </c>
       <c r="F15">
-        <v>0.003036437246963597</v>
+        <v>0.001822600243013395</v>
       </c>
       <c r="G15">
-        <v>0.003218623481781402</v>
+        <v>0.001385419936698324</v>
       </c>
       <c r="H15">
-        <v>0.002047282840654097</v>
+        <v>0.0006603789701957853</v>
       </c>
       <c r="J15">
         <v>1</v>
       </c>
       <c r="L15">
-        <v>0.795303305234591</v>
+        <v>0.6948155946454422</v>
       </c>
       <c r="M15" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="N15" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -1132,37 +1249,43 @@
         <v>22</v>
       </c>
       <c r="B16">
-        <v>0.0008434547908232725</v>
+        <v>0.0004255319148935843</v>
       </c>
       <c r="C16">
-        <v>0.001551956815114719</v>
+        <v>-0.004255319148936199</v>
       </c>
       <c r="D16">
-        <v>0.001956815114709909</v>
+        <v>0.005589307411907695</v>
       </c>
       <c r="E16">
-        <v>0.0005398110661268496</v>
+        <v>0.00498177399756985</v>
       </c>
       <c r="F16">
-        <v>0.002192982456140424</v>
+        <v>2.220446049250313E-17</v>
       </c>
       <c r="G16">
-        <v>0.001417004048583035</v>
+        <v>0.001348258835086991</v>
       </c>
       <c r="H16">
-        <v>0.000634062615969439</v>
+        <v>0.003612706424430716</v>
+      </c>
+      <c r="I16">
+        <v>1.721544765185378E-13</v>
       </c>
       <c r="J16">
-        <v>1</v>
+        <v>-7.368812583773934</v>
+      </c>
+      <c r="K16">
+        <v>1.006441555031452E-12</v>
       </c>
       <c r="L16">
-        <v>0.9496846031076999</v>
+        <v>-0.1357222686414874</v>
       </c>
       <c r="M16" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
       <c r="N16" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -1170,37 +1293,37 @@
         <v>23</v>
       </c>
       <c r="B17">
-        <v>0.002429149797570895</v>
+        <v>0.0004255319148935621</v>
       </c>
       <c r="C17">
-        <v>0.003205128205128205</v>
+        <v>0.0004863221884498281</v>
       </c>
       <c r="D17">
-        <v>0.001315789473684259</v>
+        <v>0.001215066828675582</v>
       </c>
       <c r="E17">
-        <v>6.747638326585204E-05</v>
+        <v>0.001336573511543093</v>
       </c>
       <c r="F17">
-        <v>-6.747638326581873E-05</v>
+        <v>0.002126366950182312</v>
       </c>
       <c r="G17">
-        <v>0.001390013495276678</v>
+        <v>0.001117972278748875</v>
       </c>
       <c r="H17">
-        <v>0.001284782941102986</v>
+        <v>0.00062490465801606</v>
       </c>
       <c r="J17">
         <v>1</v>
       </c>
       <c r="L17">
-        <v>0.2839907009408473</v>
+        <v>-0.6977572203804021</v>
       </c>
       <c r="M17" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="N17" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -1208,37 +1331,37 @@
         <v>24</v>
       </c>
       <c r="B18">
-        <v>0.0003373819163293157</v>
+        <v>0.001884498480243102</v>
       </c>
       <c r="C18">
-        <v>0.001417004048583004</v>
+        <v>0.0004255319148936066</v>
       </c>
       <c r="D18">
-        <v>0.002901484480431893</v>
+        <v>6.075334143380573E-05</v>
       </c>
       <c r="E18">
-        <v>0.0002024291497975561</v>
+        <v>0.001397326852976877</v>
       </c>
       <c r="F18">
-        <v>0.001349527665317185</v>
+        <v>0.001640340218712066</v>
       </c>
       <c r="G18">
-        <v>0.001241565452091791</v>
+        <v>0.001081690161651891</v>
       </c>
       <c r="H18">
-        <v>0.0009690322845353035</v>
+        <v>0.0007112064734279475</v>
       </c>
       <c r="J18">
         <v>1</v>
       </c>
       <c r="L18">
-        <v>1.115543169565771</v>
+        <v>2.2460471647153</v>
       </c>
       <c r="M18" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="N18" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -1246,37 +1369,37 @@
         <v>25</v>
       </c>
       <c r="B19">
-        <v>0.001788124156545257</v>
+        <v>0.001884498480243102</v>
       </c>
       <c r="C19">
-        <v>0.003137651821862331</v>
+        <v>0.0003039513677811523</v>
       </c>
       <c r="D19">
-        <v>-0.0001012145748987337</v>
+        <v>0.0006682867557715744</v>
       </c>
       <c r="E19">
-        <v>0.0003036437246963563</v>
+        <v>0.0003645200486026567</v>
       </c>
       <c r="F19">
-        <v>0.0009109311740891135</v>
+        <v>0.001944106925880951</v>
       </c>
       <c r="G19">
-        <v>0.001207827260458865</v>
+        <v>0.001033072715655887</v>
       </c>
       <c r="H19">
-        <v>0.001155876550896819</v>
+        <v>0.000730281941428474</v>
       </c>
       <c r="J19">
         <v>1</v>
       </c>
       <c r="L19">
-        <v>-0.9522837010469962</v>
+        <v>1.243861374465549</v>
       </c>
       <c r="M19" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="N19" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -1284,37 +1407,37 @@
         <v>26</v>
       </c>
       <c r="B20">
-        <v>0.001045883940620818</v>
+        <v>0.0009118541033433791</v>
       </c>
       <c r="C20">
-        <v>0.001417004048583004</v>
+        <v>0.0009118541033434457</v>
       </c>
       <c r="D20">
-        <v>0.0008097165991903354</v>
+        <v>0.001822600243013406</v>
       </c>
       <c r="E20">
-        <v>0.0006072874493926683</v>
+        <v>0.001579586877278194</v>
       </c>
       <c r="F20">
-        <v>0.001720647773279427</v>
+        <v>-0.0002430133657350897</v>
       </c>
       <c r="G20">
-        <v>0.00112010796221325</v>
+        <v>0.000996576392248667</v>
       </c>
       <c r="H20">
-        <v>0.0004033936620144685</v>
+        <v>0.0007173778820481561</v>
       </c>
       <c r="J20">
         <v>1</v>
       </c>
       <c r="L20">
-        <v>3.045598401257686</v>
+        <v>1.121004659495778</v>
       </c>
       <c r="M20" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="N20" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -1322,37 +1445,37 @@
         <v>27</v>
       </c>
       <c r="B21">
-        <v>0.002226720647773317</v>
+        <v>0.0008510638297871464</v>
       </c>
       <c r="C21">
-        <v>0.0009784075573549323</v>
+        <v>0.001033434650455911</v>
       </c>
       <c r="D21">
-        <v>0.001923076923076972</v>
+        <v>0.001579586877278261</v>
       </c>
       <c r="E21">
-        <v>-6.747638326585204E-05</v>
+        <v>0.0001215066828675448</v>
       </c>
       <c r="F21">
-        <v>0.0003036437246964008</v>
+        <v>0.0009113001215066974</v>
       </c>
       <c r="G21">
-        <v>0.001072874493927154</v>
+        <v>0.0008993784323791122</v>
       </c>
       <c r="H21">
-        <v>0.0008894093791757954</v>
+        <v>0.0004665223433664529</v>
       </c>
       <c r="J21">
         <v>1</v>
       </c>
       <c r="L21">
-        <v>-0.3067108024538418</v>
+        <v>1.047127861127186</v>
       </c>
       <c r="M21" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="N21" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -1360,37 +1483,37 @@
         <v>28</v>
       </c>
       <c r="B22">
-        <v>0.001113360323886681</v>
+        <v>0.0007294832826746922</v>
       </c>
       <c r="C22">
-        <v>0.00145074224021593</v>
+        <v>0.0007902735562309915</v>
       </c>
       <c r="D22">
-        <v>0.001585695006747678</v>
+        <v>0.0009720534629404698</v>
       </c>
       <c r="E22">
-        <v>0.0007422402159244168</v>
+        <v>0.0007290400972052913</v>
       </c>
       <c r="F22">
-        <v>0.0004048582995951899</v>
+        <v>0.001215066828675604</v>
       </c>
       <c r="G22">
-        <v>0.001059379217273979</v>
+        <v>0.0008871834455454099</v>
       </c>
       <c r="H22">
-        <v>0.0004386483930673402</v>
+        <v>0.0001865371916943896</v>
       </c>
       <c r="J22">
         <v>1</v>
       </c>
       <c r="L22">
-        <v>0.6224034125121716</v>
+        <v>1.365934776433885</v>
       </c>
       <c r="M22" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="N22" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -1398,37 +1521,37 @@
         <v>29</v>
       </c>
       <c r="B23">
-        <v>-3.373819163289271E-05</v>
+        <v>0.0003647416413373406</v>
       </c>
       <c r="C23">
-        <v>0.001045883940620795</v>
+        <v>0.001155015197568365</v>
       </c>
       <c r="D23">
-        <v>0.002091767881241591</v>
+        <v>0.0005467800729040406</v>
       </c>
       <c r="E23">
-        <v>0.001349527665317141</v>
+        <v>0.0007897934386390859</v>
       </c>
       <c r="F23">
-        <v>0.0001349527665317596</v>
+        <v>0.001518833535844477</v>
       </c>
       <c r="G23">
-        <v>0.0009176788124156787</v>
+        <v>0.0008750327772586618</v>
       </c>
       <c r="H23">
-        <v>0.0007873080091914129</v>
+        <v>0.0004167210574478924</v>
       </c>
       <c r="J23">
         <v>1</v>
       </c>
       <c r="L23">
-        <v>-0.7797736124013031</v>
+        <v>1.104556026788555</v>
       </c>
       <c r="M23" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="N23" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -1436,37 +1559,43 @@
         <v>30</v>
       </c>
       <c r="B24">
-        <v>-3.373819163289271E-05</v>
+        <v>-0.0001823708206687313</v>
       </c>
       <c r="C24">
-        <v>0.0007422402159244168</v>
+        <v>0.0020060790273556</v>
       </c>
       <c r="D24">
-        <v>0.00327260458839409</v>
+        <v>0.004131227217496991</v>
       </c>
       <c r="E24">
-        <v>0.0004385964912280493</v>
+        <v>-0.001215066828675604</v>
       </c>
       <c r="F24">
-        <v>0.0001349527665317707</v>
+        <v>-0.0007290400972053024</v>
       </c>
       <c r="G24">
-        <v>0.0009109311740890868</v>
+        <v>0.0008021656996605909</v>
       </c>
       <c r="H24">
-        <v>0.001210256229677316</v>
+        <v>0.001995754910590797</v>
+      </c>
+      <c r="I24">
+        <v>3.784320078197418E-06</v>
       </c>
       <c r="J24">
-        <v>1</v>
+        <v>-4.622889130738292</v>
+      </c>
+      <c r="K24">
+        <v>9.917528480793232E-06</v>
       </c>
       <c r="L24">
-        <v>-0.7960987096856016</v>
+        <v>0.0369053194320612</v>
       </c>
       <c r="M24" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
       <c r="N24" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -1474,37 +1603,37 @@
         <v>31</v>
       </c>
       <c r="B25">
-        <v>0.0007085020242915574</v>
+        <v>0.0001215805471124431</v>
       </c>
       <c r="C25">
-        <v>0.0006072874493926794</v>
+        <v>0.0008510638297872131</v>
       </c>
       <c r="D25">
-        <v>0.00131578947368427</v>
+        <v>0.001032806804374265</v>
       </c>
       <c r="E25">
-        <v>0.0008434547908231949</v>
+        <v>0.0008505467800728472</v>
       </c>
       <c r="F25">
-        <v>0.0006747638326586314</v>
+        <v>0.001032806804374253</v>
       </c>
       <c r="G25">
-        <v>0.0008299595141700667</v>
+        <v>0.0007777609531442042</v>
       </c>
       <c r="H25">
-        <v>0.0002548071199527709</v>
+        <v>0.000338035674462078</v>
       </c>
       <c r="J25">
         <v>1</v>
       </c>
       <c r="L25">
-        <v>1.63450543529154</v>
+        <v>1.074075247761809</v>
       </c>
       <c r="M25" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="N25" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -1512,37 +1641,1765 @@
         <v>32</v>
       </c>
       <c r="B26">
-        <v>0.00165317139001353</v>
+        <v>0.0007294832826746811</v>
       </c>
       <c r="C26">
-        <v>-0.0003036437246963342</v>
+        <v>0.0009118541033434569</v>
       </c>
       <c r="D26">
-        <v>0.001045883940620829</v>
+        <v>0.0009113001215067084</v>
       </c>
       <c r="E26">
-        <v>0.001214574898785425</v>
+        <v>0.0007897934386390748</v>
       </c>
       <c r="F26">
-        <v>0.0005060728744939902</v>
+        <v>0</v>
       </c>
       <c r="G26">
-        <v>0.0008232118758434881</v>
+        <v>0.0006684861892327843</v>
       </c>
       <c r="H26">
-        <v>0.0006726011225034862</v>
+        <v>0.0003416127710395953</v>
       </c>
       <c r="J26">
         <v>1</v>
       </c>
       <c r="L26">
-        <v>-0.6293349887690167</v>
+        <v>0.6446005114590878</v>
       </c>
       <c r="M26" t="s">
+        <v>78</v>
+      </c>
+      <c r="N26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N26" t="s">
+      <c r="B27">
+        <v>0.0006686930091184484</v>
+      </c>
+      <c r="C27">
+        <v>0.0006686930091185483</v>
+      </c>
+      <c r="D27">
+        <v>0.001032806804374242</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0.0009720534629404809</v>
+      </c>
+      <c r="G27">
+        <v>0.0006684492571103439</v>
+      </c>
+      <c r="H27">
+        <v>0.0003665396197431775</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>0.9875173385904411</v>
+      </c>
+      <c r="M27" t="s">
+        <v>78</v>
+      </c>
+      <c r="N27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="1" t="s">
         <v>34</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0.0010334346504559</v>
+      </c>
+      <c r="D28">
+        <v>-0.0002430133657350786</v>
+      </c>
+      <c r="E28">
+        <v>0.001215066828675537</v>
+      </c>
+      <c r="F28">
+        <v>0.00115431348724182</v>
+      </c>
+      <c r="G28">
+        <v>0.0006319603201276359</v>
+      </c>
+      <c r="H28">
+        <v>0.0006227359740027357</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>0.5541894763014242</v>
+      </c>
+      <c r="M28" t="s">
+        <v>78</v>
+      </c>
+      <c r="N28" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0.0010334346504559</v>
+      </c>
+      <c r="D29">
+        <v>-0.0002430133657350786</v>
+      </c>
+      <c r="E29">
+        <v>0.001215066828675537</v>
+      </c>
+      <c r="F29">
+        <v>0.00115431348724182</v>
+      </c>
+      <c r="G29">
+        <v>0.0006319603201276359</v>
+      </c>
+      <c r="H29">
+        <v>0.0006227359740027357</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>0.5541894763014242</v>
+      </c>
+      <c r="M29" t="s">
+        <v>78</v>
+      </c>
+      <c r="N29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0.0010334346504559</v>
+      </c>
+      <c r="D30">
+        <v>-0.0002430133657350786</v>
+      </c>
+      <c r="E30">
+        <v>0.001215066828675537</v>
+      </c>
+      <c r="F30">
+        <v>0.00115431348724182</v>
+      </c>
+      <c r="G30">
+        <v>0.0006319603201276359</v>
+      </c>
+      <c r="H30">
+        <v>0.0006227359740027357</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="L30">
+        <v>0.5541894763014242</v>
+      </c>
+      <c r="M30" t="s">
+        <v>78</v>
+      </c>
+      <c r="N30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31">
+        <v>-0.002310030395136808</v>
+      </c>
+      <c r="C31">
+        <v>-0.002978723404255379</v>
+      </c>
+      <c r="D31">
+        <v>0.008930741190765524</v>
+      </c>
+      <c r="E31">
+        <v>0.001032806804374198</v>
+      </c>
+      <c r="F31">
+        <v>-0.001640340218711977</v>
+      </c>
+      <c r="G31">
+        <v>0.0006068907954071113</v>
+      </c>
+      <c r="H31">
+        <v>0.004379109395812967</v>
+      </c>
+      <c r="I31">
+        <v>0.001453306605890771</v>
+      </c>
+      <c r="J31">
+        <v>3.183849283143014</v>
+      </c>
+      <c r="K31">
+        <v>0.002906613211781542</v>
+      </c>
+      <c r="L31">
+        <v>0.2599551167728821</v>
+      </c>
+      <c r="M31" t="s">
+        <v>78</v>
+      </c>
+      <c r="N31" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32">
+        <v>0.001094224924012077</v>
+      </c>
+      <c r="C32">
+        <v>0.001033434650455889</v>
+      </c>
+      <c r="D32">
+        <v>0.00133657351154316</v>
+      </c>
+      <c r="E32">
+        <v>0.0004252733900364291</v>
+      </c>
+      <c r="F32">
+        <v>-0.0009113001215066419</v>
+      </c>
+      <c r="G32">
+        <v>0.0005956412709081827</v>
+      </c>
+      <c r="H32">
+        <v>0.0008110643454790077</v>
+      </c>
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <v>0.4913727074059066</v>
+      </c>
+      <c r="M32" t="s">
+        <v>78</v>
+      </c>
+      <c r="N32" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33">
+        <v>0.0001823708206686647</v>
+      </c>
+      <c r="C33">
+        <v>0.001155015197568365</v>
+      </c>
+      <c r="D33">
+        <v>0.001032806804374265</v>
+      </c>
+      <c r="E33">
+        <v>0.0004860267314702127</v>
+      </c>
+      <c r="F33">
+        <v>0.0001215066828675782</v>
+      </c>
+      <c r="G33">
+        <v>0.000595545247389817</v>
+      </c>
+      <c r="H33">
+        <v>0.0004269951445272279</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="L33">
+        <v>0.5673560668151619</v>
+      </c>
+      <c r="M33" t="s">
+        <v>78</v>
+      </c>
+      <c r="N33" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34">
+        <v>0.001215805471124543</v>
+      </c>
+      <c r="C34">
+        <v>0.00133738601823703</v>
+      </c>
+      <c r="D34">
+        <v>-0.0007897934386390748</v>
+      </c>
+      <c r="E34">
+        <v>6.075334143375022E-05</v>
+      </c>
+      <c r="F34">
+        <v>0.000972053462940492</v>
+      </c>
+      <c r="G34">
+        <v>0.000559240971019348</v>
+      </c>
+      <c r="H34">
+        <v>0.000809368218561398</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="L34">
+        <v>0.2271408384217543</v>
+      </c>
+      <c r="M34" t="s">
+        <v>78</v>
+      </c>
+      <c r="N34" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35">
+        <v>0.0008510638297871464</v>
+      </c>
+      <c r="C35">
+        <v>0.0001215805471124654</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0.0009113001215066419</v>
+      </c>
+      <c r="F35">
+        <v>0.0007290400972053801</v>
+      </c>
+      <c r="G35">
+        <v>0.0005225969191223267</v>
+      </c>
+      <c r="H35">
+        <v>0.0003835416919237446</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <v>0.8979378381375254</v>
+      </c>
+      <c r="M35" t="s">
+        <v>78</v>
+      </c>
+      <c r="N35" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36">
+        <v>0.0001823708206686647</v>
+      </c>
+      <c r="C36">
+        <v>0.000668693009118515</v>
+      </c>
+      <c r="D36">
+        <v>6.075334143380573E-05</v>
+      </c>
+      <c r="E36">
+        <v>0.001154313487241754</v>
+      </c>
+      <c r="F36">
+        <v>0.0001822600243013506</v>
+      </c>
+      <c r="G36">
+        <v>0.000449678136552818</v>
+      </c>
+      <c r="H36">
+        <v>0.0004095623605726441</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="L36">
+        <v>0.4116472383636203</v>
+      </c>
+      <c r="M36" t="s">
+        <v>78</v>
+      </c>
+      <c r="N36" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37">
+        <v>0.0009118541033433791</v>
+      </c>
+      <c r="C37">
+        <v>6.079027355623268E-05</v>
+      </c>
+      <c r="D37">
+        <v>0.0003037667071689065</v>
+      </c>
+      <c r="E37">
+        <v>-1.110223024625157E-17</v>
+      </c>
+      <c r="F37">
+        <v>0.0009113001215066974</v>
+      </c>
+      <c r="G37">
+        <v>0.0004375422411150409</v>
+      </c>
+      <c r="H37">
+        <v>0.0004001748175949352</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
+      </c>
+      <c r="L37">
+        <v>0.9365447292443619</v>
+      </c>
+      <c r="M37" t="s">
+        <v>78</v>
+      </c>
+      <c r="N37" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38">
+        <v>-6.079027355626598E-05</v>
+      </c>
+      <c r="C38">
+        <v>-0.0003039513677811634</v>
+      </c>
+      <c r="D38">
+        <v>0.001215066828675593</v>
+      </c>
+      <c r="E38">
+        <v>0.0003645200486026345</v>
+      </c>
+      <c r="F38">
+        <v>0.0009113001215066863</v>
+      </c>
+      <c r="G38">
+        <v>0.0004252290714894968</v>
+      </c>
+      <c r="H38">
+        <v>0.0005712640808899363</v>
+      </c>
+      <c r="J38">
+        <v>1</v>
+      </c>
+      <c r="L38">
+        <v>-0.2207256680408913</v>
+      </c>
+      <c r="M38" t="s">
+        <v>78</v>
+      </c>
+      <c r="N38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39">
+        <v>0.0007902735562309249</v>
+      </c>
+      <c r="C39">
+        <v>-0.0007902735562310248</v>
+      </c>
+      <c r="D39">
+        <v>0.000486026731470246</v>
+      </c>
+      <c r="E39">
+        <v>0.0009720534629404143</v>
+      </c>
+      <c r="F39">
+        <v>0.0004860267314702571</v>
+      </c>
+      <c r="G39">
+        <v>0.0003888213851761635</v>
+      </c>
+      <c r="H39">
+        <v>0.0006181401364943251</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="L39">
+        <v>-0.4744206816809348</v>
+      </c>
+      <c r="M39" t="s">
+        <v>78</v>
+      </c>
+      <c r="N39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40">
+        <v>-6.079027355624378E-05</v>
+      </c>
+      <c r="C40">
+        <v>0.0001823708206686869</v>
+      </c>
+      <c r="D40">
+        <v>0.001275820170109365</v>
+      </c>
+      <c r="E40">
+        <v>0.0007897934386390971</v>
+      </c>
+      <c r="F40">
+        <v>-0.000303766707168851</v>
+      </c>
+      <c r="G40">
+        <v>0.0003766854897384108</v>
+      </c>
+      <c r="H40">
+        <v>0.0005781452719261044</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+      <c r="L40">
+        <v>1.132170353261646</v>
+      </c>
+      <c r="M40" t="s">
+        <v>78</v>
+      </c>
+      <c r="N40" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41">
+        <v>0.0007902735562309137</v>
+      </c>
+      <c r="C41">
+        <v>-0.000182370820668698</v>
+      </c>
+      <c r="D41">
+        <v>0.0004860267314702682</v>
+      </c>
+      <c r="E41">
+        <v>0.0009720534629404254</v>
+      </c>
+      <c r="F41">
+        <v>-0.0003645200486026456</v>
+      </c>
+      <c r="G41">
+        <v>0.0003402925762740527</v>
+      </c>
+      <c r="H41">
+        <v>0.0005277842375297864</v>
+      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+      <c r="L41">
+        <v>-0.3507317168461252</v>
+      </c>
+      <c r="M41" t="s">
+        <v>78</v>
+      </c>
+      <c r="N41" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42">
+        <v>0.0002431610942248974</v>
+      </c>
+      <c r="C42">
+        <v>-0.0001215805471124654</v>
+      </c>
+      <c r="D42">
+        <v>0.00036452004860269</v>
+      </c>
+      <c r="E42">
+        <v>0.0003645200486026345</v>
+      </c>
+      <c r="F42">
+        <v>0.0006682867557715966</v>
+      </c>
+      <c r="G42">
+        <v>0.0003037814800178706</v>
+      </c>
+      <c r="H42">
+        <v>0.0002548921845713894</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+      <c r="L42">
+        <v>0.6142974370664818</v>
+      </c>
+      <c r="M42" t="s">
+        <v>78</v>
+      </c>
+      <c r="N42" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43">
+        <v>0.001033434650455845</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>-6.075334143375022E-05</v>
+      </c>
+      <c r="E43">
+        <v>0.0001215066828675448</v>
+      </c>
+      <c r="F43">
+        <v>0.0003037667071689065</v>
+      </c>
+      <c r="G43">
+        <v>0.0002795909398117092</v>
+      </c>
+      <c r="H43">
+        <v>0.0003969535901084408</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+      <c r="L43">
+        <v>0.957135879786368</v>
+      </c>
+      <c r="M43" t="s">
+        <v>78</v>
+      </c>
+      <c r="N43" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B44">
+        <v>-0.0004255319148936398</v>
+      </c>
+      <c r="C44">
+        <v>-0.0002431610942249307</v>
+      </c>
+      <c r="D44">
+        <v>0.0004860267314702571</v>
+      </c>
+      <c r="E44">
+        <v>0.0007290400972053135</v>
+      </c>
+      <c r="F44">
+        <v>0.000729040097205369</v>
+      </c>
+      <c r="G44">
+        <v>0.0002550827833524738</v>
+      </c>
+      <c r="H44">
+        <v>0.0004927655643190778</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+      <c r="L44">
+        <v>-0.5734990465582734</v>
+      </c>
+      <c r="M44" t="s">
+        <v>78</v>
+      </c>
+      <c r="N44" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>0.0003039513677811523</v>
+      </c>
+      <c r="D45">
+        <v>0.000364520048602679</v>
+      </c>
+      <c r="E45">
+        <v>0.0003037667071688621</v>
+      </c>
+      <c r="F45">
+        <v>0.0002430133657351341</v>
+      </c>
+      <c r="G45">
+        <v>0.0002430502978575655</v>
+      </c>
+      <c r="H45">
+        <v>0.0001274549109891082</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="L45">
+        <v>0.4491392940315923</v>
+      </c>
+      <c r="M45" t="s">
+        <v>78</v>
+      </c>
+      <c r="N45" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46">
+        <v>0.0001215805471124431</v>
+      </c>
+      <c r="C46">
+        <v>0.0001823708206686869</v>
+      </c>
+      <c r="D46">
+        <v>0.0002430133657351341</v>
+      </c>
+      <c r="E46">
+        <v>0.0001822600243013173</v>
+      </c>
+      <c r="F46">
+        <v>0.0001215066828675671</v>
+      </c>
+      <c r="G46">
+        <v>0.0001701462881370297</v>
+      </c>
+      <c r="H46">
+        <v>4.545379015923762E-05</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+      <c r="L46">
+        <v>0.4832430508447373</v>
+      </c>
+      <c r="M46" t="s">
+        <v>78</v>
+      </c>
+      <c r="N46" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B47">
+        <v>6.079027355622157E-05</v>
+      </c>
+      <c r="C47">
+        <v>0.0001215805471124654</v>
+      </c>
+      <c r="D47">
+        <v>0.00036452004860269</v>
+      </c>
+      <c r="E47">
+        <v>6.075334143377242E-05</v>
+      </c>
+      <c r="F47">
+        <v>0.0001822600243013506</v>
+      </c>
+      <c r="G47">
+        <v>0.0001579808470013</v>
+      </c>
+      <c r="H47">
+        <v>0.0001126695144979074</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="L47">
+        <v>0.5186241440594312</v>
+      </c>
+      <c r="M47" t="s">
+        <v>78</v>
+      </c>
+      <c r="N47" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B48">
+        <v>6.079027355622157E-05</v>
+      </c>
+      <c r="C48">
+        <v>0.0001215805471124654</v>
+      </c>
+      <c r="D48">
+        <v>0.00036452004860269</v>
+      </c>
+      <c r="E48">
+        <v>6.075334143377242E-05</v>
+      </c>
+      <c r="F48">
+        <v>0.0001822600243013506</v>
+      </c>
+      <c r="G48">
+        <v>0.0001579808470013</v>
+      </c>
+      <c r="H48">
+        <v>0.0001126695144979074</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
+      <c r="L48">
+        <v>0.5186241440594312</v>
+      </c>
+      <c r="M48" t="s">
+        <v>78</v>
+      </c>
+      <c r="N48" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="A49" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B49">
+        <v>6.079027355622157E-05</v>
+      </c>
+      <c r="C49">
+        <v>0.0001215805471124654</v>
+      </c>
+      <c r="D49">
+        <v>0.00036452004860269</v>
+      </c>
+      <c r="E49">
+        <v>6.075334143377242E-05</v>
+      </c>
+      <c r="F49">
+        <v>0.0001822600243013506</v>
+      </c>
+      <c r="G49">
+        <v>0.0001579808470013</v>
+      </c>
+      <c r="H49">
+        <v>0.0001126695144979074</v>
+      </c>
+      <c r="J49">
+        <v>1</v>
+      </c>
+      <c r="L49">
+        <v>0.5186241440594312</v>
+      </c>
+      <c r="M49" t="s">
+        <v>78</v>
+      </c>
+      <c r="N49" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
+      <c r="A50" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B50">
+        <v>-0.0002431610942249307</v>
+      </c>
+      <c r="C50">
+        <v>0.0002431610942249307</v>
+      </c>
+      <c r="D50">
+        <v>-0.0001822600243013284</v>
+      </c>
+      <c r="E50">
+        <v>0.0006075334143377575</v>
+      </c>
+      <c r="F50">
+        <v>0.0003037667071689287</v>
+      </c>
+      <c r="G50">
+        <v>0.0001458080194410716</v>
+      </c>
+      <c r="H50">
+        <v>0.0003182905971599411</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+      <c r="L50">
+        <v>-0.4627348394496716</v>
+      </c>
+      <c r="M50" t="s">
+        <v>78</v>
+      </c>
+      <c r="N50" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
+      <c r="A51" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B51">
+        <v>6.079027355621047E-05</v>
+      </c>
+      <c r="C51">
+        <v>0.0007294832826747477</v>
+      </c>
+      <c r="D51">
+        <v>0.0001215066828675782</v>
+      </c>
+      <c r="E51">
+        <v>0.0001215066828675448</v>
+      </c>
+      <c r="F51">
+        <v>-0.0003645200486026235</v>
+      </c>
+      <c r="G51">
+        <v>0.0001337533746726915</v>
+      </c>
+      <c r="H51">
+        <v>0.0003489395663078388</v>
+      </c>
+      <c r="J51">
+        <v>1</v>
+      </c>
+      <c r="L51">
+        <v>0.3382893896039048</v>
+      </c>
+      <c r="M51" t="s">
+        <v>78</v>
+      </c>
+      <c r="N51" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
+      <c r="A52" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B52">
+        <v>6.079027355622157E-05</v>
+      </c>
+      <c r="C52">
+        <v>0.0001823708206686869</v>
+      </c>
+      <c r="D52">
+        <v>0.0002430133657351341</v>
+      </c>
+      <c r="E52">
+        <v>-1.110223024625157E-17</v>
+      </c>
+      <c r="F52">
+        <v>0.0001822600243013506</v>
+      </c>
+      <c r="G52">
+        <v>0.0001336868968522764</v>
+      </c>
+      <c r="H52">
+        <v>8.929485318281407E-05</v>
+      </c>
+      <c r="J52">
+        <v>1</v>
+      </c>
+      <c r="L52">
+        <v>0.5858260672346394</v>
+      </c>
+      <c r="M52" t="s">
+        <v>78</v>
+      </c>
+      <c r="N52" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
+      <c r="A53" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B53">
+        <v>-0.0003039513677811634</v>
+      </c>
+      <c r="C53">
+        <v>0.0005471124620060386</v>
+      </c>
+      <c r="D53">
+        <v>0.0006075334143378242</v>
+      </c>
+      <c r="E53">
+        <v>-0.0003645200486027123</v>
+      </c>
+      <c r="F53">
+        <v>0.0001822600243013617</v>
+      </c>
+      <c r="G53">
+        <v>0.0001336868968522697</v>
+      </c>
+      <c r="H53">
+        <v>0.0004092793617902161</v>
+      </c>
+      <c r="J53">
+        <v>1</v>
+      </c>
+      <c r="L53">
+        <v>0.6258016711118655</v>
+      </c>
+      <c r="M53" t="s">
+        <v>78</v>
+      </c>
+      <c r="N53" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14">
+      <c r="A54" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B54">
+        <v>6.079027355622157E-05</v>
+      </c>
+      <c r="C54">
+        <v>0.0002431610942249307</v>
+      </c>
+      <c r="D54">
+        <v>6.075334143379463E-05</v>
+      </c>
+      <c r="E54">
+        <v>0.0001215066828675448</v>
+      </c>
+      <c r="F54">
+        <v>0.0001215066828675671</v>
+      </c>
+      <c r="G54">
+        <v>0.0001215436149900118</v>
+      </c>
+      <c r="H54">
+        <v>6.659915891034913E-05</v>
+      </c>
+      <c r="J54">
+        <v>1</v>
+      </c>
+      <c r="L54">
+        <v>0.4445913814720843</v>
+      </c>
+      <c r="M54" t="s">
+        <v>78</v>
+      </c>
+      <c r="N54" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14">
+      <c r="A55" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B55">
+        <v>6.079027355622157E-05</v>
+      </c>
+      <c r="C55">
+        <v>0.0001215805471124654</v>
+      </c>
+      <c r="D55">
+        <v>0.0002430133657351341</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>0.0001822600243013506</v>
+      </c>
+      <c r="G55">
+        <v>0.0001215288421410343</v>
+      </c>
+      <c r="H55">
+        <v>8.591298134595425E-05</v>
+      </c>
+      <c r="J55">
+        <v>1</v>
+      </c>
+      <c r="L55">
+        <v>0.5035978302875967</v>
+      </c>
+      <c r="M55" t="s">
+        <v>78</v>
+      </c>
+      <c r="N55" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14">
+      <c r="A56" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B56">
+        <v>0.0001823708206686647</v>
+      </c>
+      <c r="C56">
+        <v>-0.0002431610942249307</v>
+      </c>
+      <c r="D56">
+        <v>2.220446049250313E-17</v>
+      </c>
+      <c r="E56">
+        <v>0.0004252733900364181</v>
+      </c>
+      <c r="F56">
+        <v>0.0001822600243013395</v>
+      </c>
+      <c r="G56">
+        <v>0.0001093486281563028</v>
+      </c>
+      <c r="H56">
+        <v>0.0002221157330353225</v>
+      </c>
+      <c r="J56">
+        <v>1</v>
+      </c>
+      <c r="L56">
+        <v>0.3727286622245273</v>
+      </c>
+      <c r="M56" t="s">
+        <v>78</v>
+      </c>
+      <c r="N56" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14">
+      <c r="A57" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57">
+        <v>0.0001823708206686647</v>
+      </c>
+      <c r="C57">
+        <v>-0.0002431610942249307</v>
+      </c>
+      <c r="D57">
+        <v>2.220446049250313E-17</v>
+      </c>
+      <c r="E57">
+        <v>0.0004252733900364181</v>
+      </c>
+      <c r="F57">
+        <v>0.0001822600243013395</v>
+      </c>
+      <c r="G57">
+        <v>0.0001093486281563028</v>
+      </c>
+      <c r="H57">
+        <v>0.0002221157330353225</v>
+      </c>
+      <c r="J57">
+        <v>1</v>
+      </c>
+      <c r="L57">
+        <v>0.3727286622245273</v>
+      </c>
+      <c r="M57" t="s">
+        <v>78</v>
+      </c>
+      <c r="N57" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14">
+      <c r="A58" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B58">
+        <v>6.079027355622157E-05</v>
+      </c>
+      <c r="C58">
+        <v>6.079027355623268E-05</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0.0001215066828675448</v>
+      </c>
+      <c r="F58">
+        <v>6.075334143378353E-05</v>
+      </c>
+      <c r="G58">
+        <v>6.076811428275652E-05</v>
+      </c>
+      <c r="H58">
+        <v>3.842379113912385E-05</v>
+      </c>
+      <c r="J58">
+        <v>1</v>
+      </c>
+      <c r="L58">
+        <v>0.520062722019066</v>
+      </c>
+      <c r="M58" t="s">
+        <v>78</v>
+      </c>
+      <c r="N58" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14">
+      <c r="A59" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B59">
+        <v>0.0001215805471124431</v>
+      </c>
+      <c r="C59">
+        <v>-6.079027355623268E-05</v>
+      </c>
+      <c r="D59">
+        <v>0.0001822600243013395</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>6.075334143378353E-05</v>
+      </c>
+      <c r="G59">
+        <v>6.076072785826669E-05</v>
+      </c>
+      <c r="H59">
+        <v>8.593909645739314E-05</v>
+      </c>
+      <c r="J59">
+        <v>1</v>
+      </c>
+      <c r="L59">
+        <v>0.4508072066060033</v>
+      </c>
+      <c r="M59" t="s">
+        <v>78</v>
+      </c>
+      <c r="N59" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
+      <c r="A60" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B60">
+        <v>0.0001215805471124431</v>
+      </c>
+      <c r="C60">
+        <v>-6.079027355623268E-05</v>
+      </c>
+      <c r="D60">
+        <v>0.0001822600243013395</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>6.075334143378353E-05</v>
+      </c>
+      <c r="G60">
+        <v>6.076072785826669E-05</v>
+      </c>
+      <c r="H60">
+        <v>8.593909645739314E-05</v>
+      </c>
+      <c r="J60">
+        <v>1</v>
+      </c>
+      <c r="L60">
+        <v>0.4508072066060033</v>
+      </c>
+      <c r="M60" t="s">
+        <v>78</v>
+      </c>
+      <c r="N60" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14">
+      <c r="A61" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B61">
+        <v>0.0001215805471124431</v>
+      </c>
+      <c r="C61">
+        <v>-6.079027355623268E-05</v>
+      </c>
+      <c r="D61">
+        <v>0.0001822600243013395</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>6.075334143378353E-05</v>
+      </c>
+      <c r="G61">
+        <v>6.076072785826669E-05</v>
+      </c>
+      <c r="H61">
+        <v>8.593909645739314E-05</v>
+      </c>
+      <c r="J61">
+        <v>1</v>
+      </c>
+      <c r="L61">
+        <v>0.4508072066060033</v>
+      </c>
+      <c r="M61" t="s">
+        <v>78</v>
+      </c>
+      <c r="N61" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14">
+      <c r="A62" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B62">
+        <v>-0.0003039513677811856</v>
+      </c>
+      <c r="C62">
+        <v>6.079027355622157E-05</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0.0005467800729039741</v>
+      </c>
+      <c r="F62">
+        <v>-6.075334143373912E-05</v>
+      </c>
+      <c r="G62">
+        <v>4.857312744905418E-05</v>
+      </c>
+      <c r="H62">
+        <v>0.0002781886282379001</v>
+      </c>
+      <c r="J62">
+        <v>1</v>
+      </c>
+      <c r="L62">
+        <v>0.8930719933708199</v>
+      </c>
+      <c r="M62" t="s">
+        <v>78</v>
+      </c>
+      <c r="N62" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14">
+      <c r="A63" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B63">
+        <v>0.000425531914893551</v>
+      </c>
+      <c r="C63">
+        <v>-0.0001215805471124654</v>
+      </c>
+      <c r="D63">
+        <v>-6.075334143377242E-05</v>
+      </c>
+      <c r="E63">
+        <v>0.0001822600243013173</v>
+      </c>
+      <c r="F63">
+        <v>-0.0002430133657351008</v>
+      </c>
+      <c r="G63">
+        <v>3.648893698270595E-05</v>
+      </c>
+      <c r="H63">
+        <v>0.0002388167533059967</v>
+      </c>
+      <c r="J63">
+        <v>1</v>
+      </c>
+      <c r="L63">
+        <v>-0.6521718942835801</v>
+      </c>
+      <c r="M63" t="s">
+        <v>78</v>
+      </c>
+      <c r="N63" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14">
+      <c r="A64" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B64">
+        <v>-0.001215805471124654</v>
+      </c>
+      <c r="C64">
+        <v>-0.0003039513677811634</v>
+      </c>
+      <c r="D64">
+        <v>0.0003645200486027123</v>
+      </c>
+      <c r="E64">
+        <v>0.001458080194410649</v>
+      </c>
+      <c r="F64">
+        <v>-0.0004252733900364291</v>
+      </c>
+      <c r="G64">
+        <v>-2.448599718577695E-05</v>
+      </c>
+      <c r="H64">
+        <v>0.0008952431773256659</v>
+      </c>
+      <c r="I64">
+        <v>1.439896341360007E-09</v>
+      </c>
+      <c r="J64">
+        <v>-6.050955039134048</v>
+      </c>
+      <c r="K64">
+        <v>5.21105342587431E-09</v>
+      </c>
+      <c r="L64">
+        <v>0.04506049654468152</v>
+      </c>
+      <c r="M64" t="s">
+        <v>79</v>
+      </c>
+      <c r="N64" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14">
+      <c r="A65" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B65">
+        <v>0.000790273556230936</v>
+      </c>
+      <c r="C65">
+        <v>-0.0005471124620060941</v>
+      </c>
+      <c r="D65">
+        <v>6.075334143378353E-05</v>
+      </c>
+      <c r="E65">
+        <v>-0.0009113001215067196</v>
+      </c>
+      <c r="F65">
+        <v>4.440892098500626E-17</v>
+      </c>
+      <c r="G65">
+        <v>-0.00012147713716961</v>
+      </c>
+      <c r="H65">
+        <v>0.0005803860345389387</v>
+      </c>
+      <c r="J65">
+        <v>1</v>
+      </c>
+      <c r="L65">
+        <v>0.5272337975919879</v>
+      </c>
+      <c r="M65" t="s">
+        <v>78</v>
+      </c>
+      <c r="N65" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14">
+      <c r="A66" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B66">
+        <v>0.0001215805471124431</v>
+      </c>
+      <c r="C66">
+        <v>-0.0009726443768997229</v>
+      </c>
+      <c r="D66">
+        <v>0.0003037667071689176</v>
+      </c>
+      <c r="E66">
+        <v>0.0005467800729039741</v>
+      </c>
+      <c r="F66">
+        <v>-0.0007897934386390859</v>
+      </c>
+      <c r="G66">
+        <v>-0.0001580620976706948</v>
+      </c>
+      <c r="H66">
+        <v>0.0006084270072863274</v>
+      </c>
+      <c r="J66">
+        <v>1</v>
+      </c>
+      <c r="L66">
+        <v>0.2711087940477009</v>
+      </c>
+      <c r="M66" t="s">
+        <v>78</v>
+      </c>
+      <c r="N66" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14">
+      <c r="A67" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B67">
+        <v>-0.0004863221884498725</v>
+      </c>
+      <c r="C67">
+        <v>-0.0002431610942249307</v>
+      </c>
+      <c r="D67">
+        <v>-0.0001215066828675448</v>
+      </c>
+      <c r="E67">
+        <v>-0.0002430133657351341</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>-0.0002188006662554964</v>
+      </c>
+      <c r="H67">
+        <v>0.0001612992875752931</v>
+      </c>
+      <c r="J67">
+        <v>1</v>
+      </c>
+      <c r="L67">
+        <v>-0.1985672646896087</v>
+      </c>
+      <c r="M67" t="s">
+        <v>78</v>
+      </c>
+      <c r="N67" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14">
+      <c r="A68" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B68">
+        <v>-0.0004255319148936621</v>
+      </c>
+      <c r="C68">
+        <v>-0.002188449848024365</v>
+      </c>
+      <c r="D68">
+        <v>0.001458080194410716</v>
+      </c>
+      <c r="E68">
+        <v>0.0006682867557715521</v>
+      </c>
+      <c r="F68">
+        <v>-0.00145808019441066</v>
+      </c>
+      <c r="G68">
+        <v>-0.0003891390014292839</v>
+      </c>
+      <c r="H68">
+        <v>0.001335054098555495</v>
+      </c>
+      <c r="J68">
+        <v>1</v>
+      </c>
+      <c r="L68">
+        <v>0.572559384578174</v>
+      </c>
+      <c r="M68" t="s">
+        <v>78</v>
+      </c>
+      <c r="N68" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14">
+      <c r="A69" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B69">
+        <v>-0.0006079027355623268</v>
+      </c>
+      <c r="C69">
+        <v>-0.0003039513677811745</v>
+      </c>
+      <c r="D69">
+        <v>-0.0004252733900364291</v>
+      </c>
+      <c r="E69">
+        <v>-0.0004252733900364736</v>
+      </c>
+      <c r="F69">
+        <v>-0.0004860267314701905</v>
+      </c>
+      <c r="G69">
+        <v>-0.0004496855229773189</v>
+      </c>
+      <c r="H69">
+        <v>9.877623019033579E-05</v>
+      </c>
+      <c r="J69">
+        <v>1</v>
+      </c>
+      <c r="L69">
+        <v>-0.7071815735419842</v>
+      </c>
+      <c r="M69" t="s">
+        <v>78</v>
+      </c>
+      <c r="N69" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14">
+      <c r="A70" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B70">
+        <v>-0.001094224924012199</v>
+      </c>
+      <c r="C70">
+        <v>-0.00279635258358667</v>
+      </c>
+      <c r="D70">
+        <v>0.002733900364520081</v>
+      </c>
+      <c r="E70">
+        <v>0.0003645200486026567</v>
+      </c>
+      <c r="F70">
+        <v>-0.003341433778857794</v>
+      </c>
+      <c r="G70">
+        <v>-0.0008267181746667851</v>
+      </c>
+      <c r="H70">
+        <v>0.002207798316055506</v>
+      </c>
+      <c r="I70">
+        <v>2.030756628323266E-66</v>
+      </c>
+      <c r="J70">
+        <v>17.21553125936445</v>
+      </c>
+      <c r="K70">
+        <v>1.543375037525682E-64</v>
+      </c>
+      <c r="L70">
+        <v>0.3829471881868348</v>
+      </c>
+      <c r="M70" t="s">
+        <v>78</v>
+      </c>
+      <c r="N70" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14">
+      <c r="A71" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B71">
+        <v>-0.001823708206686969</v>
+      </c>
+      <c r="C71">
+        <v>-0.002249240121580598</v>
+      </c>
+      <c r="D71">
+        <v>0.0006682867557715966</v>
+      </c>
+      <c r="E71">
+        <v>-0.001944106925880962</v>
+      </c>
+      <c r="F71">
+        <v>-0.003219927095990238</v>
+      </c>
+      <c r="G71">
+        <v>-0.001713739118873434</v>
+      </c>
+      <c r="H71">
+        <v>0.00128798861334796</v>
+      </c>
+      <c r="J71">
+        <v>1</v>
+      </c>
+      <c r="L71">
+        <v>0.7297202547936362</v>
+      </c>
+      <c r="M71" t="s">
+        <v>78</v>
+      </c>
+      <c r="N71" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>